<commit_message>
Storing link indices and value format
Not doing anything with them yet, but they are there in the model
components, namely Link and Node.
</commit_message>
<xml_diff>
--- a/optima/standard-test-data-transit-test.xlsx
+++ b/optima/standard-test-data-transit-test.xlsx
@@ -2761,7 +2761,7 @@
   <dimension ref="A1:AI374"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3039,7 +3039,7 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -3438,7 +3438,7 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>0.1</v>
+        <v>0.6</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Significant change to compartment indexing
A ModelCompartment index is now expected to be a tuple, with first
element as its corresponding ModelPopulation index.
Accordingly, links will contain tuples as their index_to and index_from
attributes, allowing for inter-population links to be stored in the same
list as intra-population links and still be distinguished.
All transfer (i.e. migration) links are thus now stored in their
'source' population. This will allow all transitions to be applied
simultaneously.
However, this raises a few potential issues in terms of the getComp()
function, so function printLinkVars() is currently commented out.
Function stepCascadeForward() also forces a crash if any
inter-population links are found in the relevant population.
</commit_message>
<xml_diff>
--- a/optima/standard-test-data-transit-test.xlsx
+++ b/optima/standard-test-data-transit-test.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Population Definitions" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="91">
   <si>
     <t>Name</t>
   </si>
@@ -287,6 +287,9 @@
   </si>
   <si>
     <t>Death Rate (Other Causes)</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
 </sst>
 </file>
@@ -627,7 +630,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -655,6 +660,12 @@
       <c r="B2" t="str">
         <f>LEFT(A2,3)&amp;"1"</f>
         <v>Pop1</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
+      </c>
+      <c r="D2">
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
@@ -684,7 +695,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -714,7 +727,7 @@
         <v>Pop1</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -2760,8 +2773,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI374"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3039,7 +3052,7 @@
         <v>13</v>
       </c>
       <c r="C4">
-        <v>0.7</v>
+        <v>0.2</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -3438,7 +3451,7 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>0.6</v>
+        <v>0.1</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
Fraction and Probability reconciliation
First success in dealing with transition rates that are given either as
a yearly 'fraction' of compartment size or a yearly independent
'probability' of a compartment member moving.
Conversion from one size of timestep dt to another also appears to be
working.
So, as an example, two outflows with yearly movement probabilities of
0.2 and 0.1 will produce dt-based values commensurate with actual yearly
fractions of ~1.9 and ~0.09, whereas two outflows with yearly movement
fractions 0.2 and 0.1 will produce values commensurate with actual
yearly fractions 0.2 and 0.1.
It follows that a fraction of 0.7 and a probability of 0.4 will
correspond to values commensurate with fractions 0.7 and ~0.2. But if
both are entered as fractions, the numerical conversion procedure should
crash (i.e. negative population problem).
This is a complicated concept and extremely damaging to performance.
Requires more thought to maintain this level of rigour.
</commit_message>
<xml_diff>
--- a/optima/standard-test-data-transit-test.xlsx
+++ b/optima/standard-test-data-transit-test.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -290,6 +290,9 @@
   </si>
   <si>
     <t>y</t>
+  </si>
+  <si>
+    <t>Fraction</t>
   </si>
 </sst>
 </file>
@@ -2773,8 +2776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI374"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3049,10 +3052,10 @@
         <v>Population 3</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>91</v>
       </c>
       <c r="C4">
-        <v>0.2</v>
+        <v>0.7</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -3451,7 +3454,7 @@
         <v>13</v>
       </c>
       <c r="C9">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="D9" t="s">
         <v>14</v>

</xml_diff>